<commit_message>
alterações na logica de distribuição
</commit_message>
<xml_diff>
--- a/processosdistribuidos_completos.xlsx
+++ b/processosdistribuidos_completos.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024/103421.1</t>
+          <t>2024/193641.3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -485,14 +485,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pessoa1</t>
+          <t>Fulano2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024/103441.1</t>
+          <t>2024/152522.1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -501,23 +501,23 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45634</v>
+        <v>45602</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SANDERLAN</t>
+          <t>MARCOS</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pessoa3</t>
+          <t>Fulano2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024/103422.1</t>
+          <t>2024/113415.2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,23 +526,24 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45602</v>
+        <v>45397</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>MARCOS</t>
+          <t>SABRINA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Pessoa1</t>
+          <t xml:space="preserve">Fulano1
+</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024/103415.1</t>
+          <t>2024/193641.4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -551,23 +552,23 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45397</v>
+        <v>45634</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>SABRINA</t>
+          <t>SANDERLAN</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pessoa2</t>
+          <t>Fulano6</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024/193641.1</t>
+          <t>2024/152522.5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -576,23 +577,23 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45634</v>
+        <v>45602</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SANDERLAN</t>
+          <t>MARCOS</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pessoa1</t>
+          <t>Fulano3</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024/152422.1</t>
+          <t>2024/173425.7</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -601,23 +602,23 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45602</v>
+        <v>45397</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>MARCOS</t>
+          <t>SABRINA</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pessoa3</t>
+          <t>Fulano6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024/113415.1</t>
+          <t>2024/193821.3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -626,23 +627,23 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45397</v>
+        <v>45634</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SABRINA</t>
+          <t>SANDERLAN</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Pessoa2</t>
+          <t>Fulano3</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024/193641.3</t>
+          <t>2024/152522.8</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -651,23 +652,23 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45634</v>
+        <v>45602</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>SANDERLAN</t>
+          <t>MARCOS</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Pessoa3</t>
+          <t>Fulano5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024/152522.1</t>
+          <t>2024/113415.5</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -676,23 +677,24 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45602</v>
+        <v>45397</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>MARCOS</t>
+          <t>SABRINA</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Pessoa1</t>
+          <t xml:space="preserve">Fulano4
+</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024/113415.2</t>
+          <t>2024/196641.3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -701,16 +703,68 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
+        <v>45634</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>SANDERLAN</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fulano4
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024/122522.9</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45602</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>MARCOS</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fulano1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024/119605.2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
         <v>45397</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>SABRINA</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Pessoa2</t>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Fulano5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando inserts separados para cada processo
</commit_message>
<xml_diff>
--- a/processosdistribuidos_completos.xlsx
+++ b/processosdistribuidos_completos.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -768,6 +768,58 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024/109609.5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45390</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>SANDERLAN</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fulano1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024/029609.9</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45390</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>MARCOS</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fulano4
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando opções para o usuario limitar a quantidade de processos distribuidos
</commit_message>
<xml_diff>
--- a/processosdistribuidos_completos.xlsx
+++ b/processosdistribuidos_completos.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024/193641.3</t>
+          <t>2024/112521.7</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45634</v>
+        <v>45331</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -485,14 +485,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Fulano2</t>
+          <t>Fulano5</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024/152522.1</t>
+          <t>2024/113511.8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45602</v>
+        <v>45355</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -517,7 +517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024/113415.2</t>
+          <t>2024/113381.2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45397</v>
+        <v>45355</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -543,7 +543,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024/193641.4</t>
+          <t>2024/112385.2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45634</v>
+        <v>45579</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -561,14 +561,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Fulano6</t>
+          <t>Fulano3</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024/152522.5</t>
+          <t>2024/413385.6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45602</v>
+        <v>45576</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -586,14 +586,15 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Fulano3</t>
+          <t xml:space="preserve">Fulano4
+</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024/173425.7</t>
+          <t>2024/553362.6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -602,23 +603,23 @@
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45397</v>
+        <v>45576</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>SABRINA</t>
+          <t>YGOR</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Fulano6</t>
+          <t>Fulano2</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024/193821.3</t>
+          <t>2024/955322.1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -627,23 +628,24 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45634</v>
+        <v>45576</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>SANDERLAN</t>
+          <t>EDUARDO</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Fulano3</t>
+          <t xml:space="preserve">Fulano1
+</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024/152522.8</t>
+          <t>2024/193641.3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -652,171 +654,398 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45602</v>
+        <v>45634</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MARCOS</t>
+          <t>SANDERLAN</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Fulano5</t>
+          <t>Fulano2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>2024/152522.1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>45602</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>MARCOS</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Fulano2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024/113415.2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>45397</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fulano1
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024/193641.4</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>45634</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>SANDERLAN</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Fulano6</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024/152522.5</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>45602</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>MARCOS</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Fulano3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024/173425.7</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>45397</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>SABRINA</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Fulano6</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024/193821.3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>45634</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>SANDERLAN</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Fulano3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024/152522.8</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>45602</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>MARCOS</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Fulano5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>2024/113415.5</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>SECRETARIA 2-B</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="n">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
         <v>45397</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>SABRINA</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t xml:space="preserve">Fulano4
 </t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="18">
+      <c r="A18" t="inlineStr">
         <is>
           <t>2024/196641.3</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SECRETARIA 2-B</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
         <v>45634</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>SANDERLAN</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t xml:space="preserve">Fulano4
 </t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>2024/122522.9</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SECRETARIA 2-B</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="n">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
         <v>45602</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>MARCOS</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t xml:space="preserve">Fulano1
 </t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>2024/119605.2</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>SECRETARIA 2-B</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="n">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
         <v>45397</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>SABRINA</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>Fulano5</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="21">
+      <c r="A21" t="inlineStr">
         <is>
           <t>2024/109609.5</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>SECRETARIA 2-B</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="n">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
         <v>45390</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>SANDERLAN</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t xml:space="preserve">Fulano1
 </t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
         <is>
           <t>2024/029609.9</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>SECRETARIA 2-B</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="n">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
         <v>45390</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>MARCOS</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t xml:space="preserve">Fulano4
 </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2024/015609.9</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45391</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>RUY</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fulano4
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2024/112521.8</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SECRETARIA 2-B</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45331</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>SANDERLAN</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Fulano3</t>
         </is>
       </c>
     </row>

</xml_diff>